<commit_message>
Assignment 7 Factor Snalysis
</commit_message>
<xml_diff>
--- a/EigenValues_PC_Selection_Seshadri.xlsx
+++ b/EigenValues_PC_Selection_Seshadri.xlsx
@@ -147,9 +147,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -162,11 +166,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -459,11 +467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1222313984"/>
-        <c:axId val="1222311664"/>
+        <c:axId val="1222287040"/>
+        <c:axId val="1219267552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1222313984"/>
+        <c:axId val="1222287040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,12 +583,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1222311664"/>
+        <c:crossAx val="1219267552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1222311664"/>
+        <c:axId val="1219267552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9.0"/>
@@ -693,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1222313984"/>
+        <c:crossAx val="1222287040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1308,10 +1316,10 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>